<commit_message>
Ajout de Use cases + Création d'un MCD
</commit_message>
<xml_diff>
--- a/Documentation/Use cases.xlsx
+++ b/Documentation/Use cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Use case 1</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Le joueur appuie sur le bouton "&gt;" .</t>
   </si>
   <si>
-    <t>La carte "2" disparait la carte "1" devient la carte "2" et la prochaine carte de la pile apparaît à l'endroit de la carte "1".</t>
-  </si>
-  <si>
     <t>Use case 4</t>
   </si>
   <si>
@@ -61,6 +58,27 @@
   </si>
   <si>
     <t>Une nouvelle partie commence, le score du joueur est remis à 0.</t>
+  </si>
+  <si>
+    <t>La carte "2" disparait, la carte "1" devient la carte "2" et la prochaine carte de la pile apparaît à l'endroit de la carte "1".</t>
+  </si>
+  <si>
+    <t>Le joueur réussi à éliminer toutes les cartes formant une pyramide.</t>
+  </si>
+  <si>
+    <t>Une nouvelle pyramide apparait et la partie continue</t>
+  </si>
+  <si>
+    <t>Le joueur à n'a plus aucune "donne" (Redistribution de la pyramide)</t>
+  </si>
+  <si>
+    <t>La partie se termine. Le système lui demande un nom d'utilisateur et associe ce dernier à son score qui est stocké dans une base de données</t>
+  </si>
+  <si>
+    <t>Use case 5</t>
+  </si>
+  <si>
+    <t>Use case 6</t>
   </si>
 </sst>
 </file>
@@ -194,12 +212,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -214,6 +226,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D18"/>
+  <dimension ref="C3:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,102 +527,150 @@
   <sheetData>
     <row r="3" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>10</v>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
+      <c r="D18" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>13</v>
+    <row r="22" spans="3:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>